<commit_message>
Aktualisieren der README und Progress bar verschönern
Progressbar zu Präsentation hinzugefügt. Mockup erstellt und Planung.docx aktualisiert.
</commit_message>
<xml_diff>
--- a/Dokumentation/Arbeitszeit.xlsx
+++ b/Dokumentation/Arbeitszeit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Daten\Android_Apps\Notification-Demo\Dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2885E705-8804-4678-BFA5-825196FECEB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CDA214C-826E-4BB7-9E7F-58744B28FCFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Datum</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>issue #3</t>
+  </si>
+  <si>
+    <t>Präsentation, Verschönerungen und README</t>
   </si>
 </sst>
 </file>
@@ -423,15 +426,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -491,6 +493,17 @@
         <v>4</v>
       </c>
     </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>44499</v>
+      </c>
+      <c r="B7" s="8">
+        <v>1.45</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Big-Picture Style Notification implementieren
Aussehen minimal verändert(launcherIcon), Präsentation weiter erstellt.
</commit_message>
<xml_diff>
--- a/Dokumentation/Arbeitszeit.xlsx
+++ b/Dokumentation/Arbeitszeit.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Daten\Android_Apps\Notification-Demo\Dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CDA214C-826E-4BB7-9E7F-58744B28FCFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61B6BC5E-50FB-4926-A50E-D73D6E9AA068}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Datum</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>Präsentation, Verschönerungen und README</t>
+  </si>
+  <si>
+    <t>Präsentation, Aussehen, Big-Picture</t>
   </si>
 </sst>
 </file>
@@ -426,9 +429,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="A8:B8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -504,6 +509,17 @@
         <v>5</v>
       </c>
     </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>44501</v>
+      </c>
+      <c r="B8" s="8">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Big Text Style implementiert
Testen ob NotificationController umgebaut werden kann.
</commit_message>
<xml_diff>
--- a/Dokumentation/Arbeitszeit.xlsx
+++ b/Dokumentation/Arbeitszeit.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Daten\Android_Apps\Notification-Demo\Dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A22E0CEC-70BE-44ED-9575-81583C379CF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64E9438A-037B-47C1-97D1-1733273CAC70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3765" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Datum</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>UI überarbeiten, Auswahl der Notifications</t>
+  </si>
+  <si>
+    <t>UI Bug fixen und Media Kontrollen Notification</t>
   </si>
 </sst>
 </file>
@@ -72,7 +75,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -138,11 +141,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -152,6 +166,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -432,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -534,6 +549,17 @@
         <v>7</v>
       </c>
     </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>44509</v>
+      </c>
+      <c r="B10" s="9">
+        <v>2.36</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Gliederung der Projektarbeit hinzugefügt
</commit_message>
<xml_diff>
--- a/Dokumentation/Arbeitszeit.xlsx
+++ b/Dokumentation/Arbeitszeit.xlsx
@@ -8,24 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Daten\Android_Apps\Notification-Demo\Dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{439A534A-227A-4A80-819E-5AB5110ED217}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA49F13E-BBA6-468E-BD8E-AD070418B097}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3765" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Datum</t>
   </si>
@@ -70,6 +79,9 @@
   </si>
   <si>
     <t>Präsentation und Dokumentation</t>
+  </si>
+  <si>
+    <t>Summe</t>
   </si>
 </sst>
 </file>
@@ -93,7 +105,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -159,11 +171,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -173,6 +198,8 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -453,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -621,15 +648,24 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="4">
+    <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="9">
         <v>44529</v>
       </c>
-      <c r="B16" s="8">
+      <c r="B16" s="10">
         <v>2</v>
       </c>
       <c r="C16" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="7">
+        <f>SUM(B2:B16)</f>
+        <v>29.479999999999997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Einbauen des simulierten Pausierens des Medien Inhaltes.
</commit_message>
<xml_diff>
--- a/Dokumentation/Arbeitszeit.xlsx
+++ b/Dokumentation/Arbeitszeit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Daten\Android_Apps\Notification-Demo\Dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD283CB2-C958-46B6-BD12-2DFE2ED2D8D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF3DBB58-14BB-46D5-BEA5-D02F1D5C48A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -196,16 +196,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -488,8 +486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -518,13 +516,13 @@
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="7"/>
+      <c r="C2" s="6"/>
       <c r="D2" s="4" t="s">
         <v>21</v>
       </c>
       <c r="E2" s="5">
         <f>SUM(B3:B21)</f>
-        <v>44.48</v>
+        <v>48.48</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>0</v>
@@ -541,9 +539,7 @@
       <c r="B3" s="3">
         <v>2</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
+      <c r="C3" s="6"/>
       <c r="G3" s="2">
         <v>44565</v>
       </c>
@@ -561,9 +557,7 @@
       <c r="B4" s="3">
         <v>3</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
+      <c r="C4" s="6"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
@@ -572,11 +566,9 @@
       <c r="B5" s="3">
         <v>0.42</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
@@ -585,11 +577,9 @@
       <c r="B6" s="3">
         <v>0.45</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
@@ -598,11 +588,9 @@
       <c r="B7" s="3">
         <v>2.2999999999999998</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
@@ -611,11 +599,9 @@
       <c r="B8" s="3">
         <v>1.45</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
@@ -624,11 +610,9 @@
       <c r="B9" s="3">
         <v>2</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
@@ -637,11 +621,9 @@
       <c r="B10" s="3">
         <v>2</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
@@ -650,11 +632,9 @@
       <c r="B11" s="3">
         <v>2.36</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
@@ -663,11 +643,9 @@
       <c r="B12" s="3">
         <v>4</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
@@ -676,11 +654,9 @@
       <c r="B13" s="3">
         <v>1.5</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
@@ -689,11 +665,9 @@
       <c r="B14" s="3">
         <v>1</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
@@ -702,11 +676,9 @@
       <c r="B15" s="3">
         <v>3</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
@@ -715,72 +687,62 @@
       <c r="B16" s="3">
         <v>2</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>44529</v>
       </c>
       <c r="B17" s="3">
         <v>2</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>44899</v>
       </c>
       <c r="B18" s="3">
         <v>2</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>44907</v>
       </c>
       <c r="B19" s="3">
         <v>5</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>44922</v>
       </c>
       <c r="B20" s="3">
         <v>4</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>44925</v>
       </c>
-      <c r="B21" s="8">
-        <v>4</v>
-      </c>
-      <c r="C21" s="8" t="s">
+      <c r="B21" s="3">
+        <v>8</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Einbinden eines Dialogs zur Erklärung der Berechtigungsanfrage.
</commit_message>
<xml_diff>
--- a/Dokumentation/Arbeitszeit.xlsx
+++ b/Dokumentation/Arbeitszeit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Daten\Android_Apps\Notification-Demo\Dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF3DBB58-14BB-46D5-BEA5-D02F1D5C48A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A01BCA1A-4956-4070-B0EC-0DE4764556E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -487,7 +487,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -522,7 +522,7 @@
       </c>
       <c r="E2" s="5">
         <f>SUM(B3:B21)</f>
-        <v>48.48</v>
+        <v>50.48</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>0</v>
@@ -740,7 +740,7 @@
         <v>44925</v>
       </c>
       <c r="B21" s="3">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
Einbauen eines Dialogs tur Erklärung der Berechtigungen.
README aktualisiert
</commit_message>
<xml_diff>
--- a/Dokumentation/Arbeitszeit.xlsx
+++ b/Dokumentation/Arbeitszeit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Daten\Android_Apps\Notification-Demo\Dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A01BCA1A-4956-4070-B0EC-0DE4764556E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59AC4BA0-5E0B-4466-A775-C0E88ECDCF17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>Datum</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t>Umbau auf Singleton der Application Klasse und Öffnen der App Einst.</t>
+  </si>
+  <si>
+    <t>Beheben des "System UI stopped" fehlers und Dialog für Berechtig.</t>
   </si>
 </sst>
 </file>
@@ -126,7 +129,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -150,10 +153,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="medium">
@@ -165,29 +168,14 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
+      <left/>
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -196,14 +184,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -484,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -516,13 +503,13 @@
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="4" t="s">
+      <c r="C2" s="3"/>
+      <c r="D2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="5">
-        <f>SUM(B3:B21)</f>
-        <v>50.48</v>
+      <c r="E2" s="4">
+        <f>SUM(B:B)</f>
+        <v>53.48</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>0</v>
@@ -539,7 +526,7 @@
       <c r="B3" s="3">
         <v>2</v>
       </c>
-      <c r="C3" s="6"/>
+      <c r="C3" s="3"/>
       <c r="G3" s="2">
         <v>44565</v>
       </c>
@@ -557,7 +544,7 @@
       <c r="B4" s="3">
         <v>3</v>
       </c>
-      <c r="C4" s="6"/>
+      <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
@@ -566,7 +553,7 @@
       <c r="B5" s="3">
         <v>0.42</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="3" t="s">
         <v>2</v>
       </c>
     </row>
@@ -577,7 +564,7 @@
       <c r="B6" s="3">
         <v>0.45</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="3" t="s">
         <v>3</v>
       </c>
     </row>
@@ -588,7 +575,7 @@
       <c r="B7" s="3">
         <v>2.2999999999999998</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="3" t="s">
         <v>4</v>
       </c>
     </row>
@@ -599,7 +586,7 @@
       <c r="B8" s="3">
         <v>1.45</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="3" t="s">
         <v>5</v>
       </c>
     </row>
@@ -610,7 +597,7 @@
       <c r="B9" s="3">
         <v>2</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -621,7 +608,7 @@
       <c r="B10" s="3">
         <v>2</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="3" t="s">
         <v>7</v>
       </c>
     </row>
@@ -632,7 +619,7 @@
       <c r="B11" s="3">
         <v>2.36</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -643,7 +630,7 @@
       <c r="B12" s="3">
         <v>4</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -654,7 +641,7 @@
       <c r="B13" s="3">
         <v>1.5</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="3" t="s">
         <v>10</v>
       </c>
     </row>
@@ -665,7 +652,7 @@
       <c r="B14" s="3">
         <v>1</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="3" t="s">
         <v>11</v>
       </c>
     </row>
@@ -676,7 +663,7 @@
       <c r="B15" s="3">
         <v>3</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="3" t="s">
         <v>12</v>
       </c>
     </row>
@@ -687,7 +674,7 @@
       <c r="B16" s="3">
         <v>2</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="3" t="s">
         <v>13</v>
       </c>
     </row>
@@ -698,7 +685,7 @@
       <c r="B17" s="3">
         <v>2</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="3" t="s">
         <v>14</v>
       </c>
     </row>
@@ -709,7 +696,7 @@
       <c r="B18" s="3">
         <v>2</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -720,7 +707,7 @@
       <c r="B19" s="3">
         <v>5</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="3" t="s">
         <v>19</v>
       </c>
     </row>
@@ -731,7 +718,7 @@
       <c r="B20" s="3">
         <v>4</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="3" t="s">
         <v>20</v>
       </c>
     </row>
@@ -744,6 +731,17 @@
       </c>
       <c r="C21" s="3" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>44930</v>
+      </c>
+      <c r="B22" s="3">
+        <v>3</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Aktualisieren der Lizenzverweiße in den Dateien.
Die Verweise in den Quelldateien sind jetzt nach den offiziellen Empfehlungen der GNU. Entfernen Benutzerspezifischer Android Studio Einstellungen.
</commit_message>
<xml_diff>
--- a/Dokumentation/Arbeitszeit.xlsx
+++ b/Dokumentation/Arbeitszeit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Daten\Android_Apps\Notification-Demo\Dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59AC4BA0-5E0B-4466-A775-C0E88ECDCF17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59789416-7248-4C2C-8AB9-613F3EC26BA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -473,8 +473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,7 +509,7 @@
       </c>
       <c r="E2" s="4">
         <f>SUM(B:B)</f>
-        <v>53.48</v>
+        <v>54.48</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>0</v>
@@ -738,7 +738,7 @@
         <v>44930</v>
       </c>
       <c r="B22" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>23</v>

</xml_diff>